<commit_message>
Finished correcting/verifying the orientations of JLCPCB sourced components.
</commit_message>
<xml_diff>
--- a/driver_40mm_atmega_v1p9/production/rev1/CPL_JLCPCB_driver_v1p9_rev1.xlsx
+++ b/driver_40mm_atmega_v1p9/production/rev1/CPL_JLCPCB_driver_v1p9_rev1.xlsx
@@ -2052,7 +2052,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2067,6 +2067,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2088,8 +2096,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2135,7 +2143,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2160,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,7 +2177,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2186,7 +2194,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,7 +2755,7 @@
         <v>8</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2764,7 +2772,7 @@
         <v>8</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2781,7 +2789,7 @@
         <v>8</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,414 +2806,414 @@
         <v>8</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="42" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="2" t="n">
+      <c r="D42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+    <row r="43" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="2" t="n">
+      <c r="D43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+    <row r="44" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="2" t="n">
+      <c r="D44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+    <row r="45" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="2" t="n">
+      <c r="D45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+    <row r="46" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="2" t="n">
+      <c r="D46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
+    <row r="47" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="2" t="n">
+      <c r="D47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+    <row r="48" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="2" t="n">
+      <c r="D48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
+    <row r="49" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="2" t="n">
+      <c r="D49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
+    <row r="50" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="2" t="n">
+      <c r="D50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
+    <row r="51" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="2" t="n">
+      <c r="D51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
+    <row r="52" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="2" t="n">
+      <c r="D52" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="s">
+    <row r="53" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="2" t="n">
+      <c r="D53" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
+    <row r="54" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="2" t="n">
+      <c r="D54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="s">
+    <row r="55" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="2" t="n">
+      <c r="D55" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
+    <row r="56" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="2" t="n">
+      <c r="D56" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
+    <row r="57" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="2" t="n">
+      <c r="D57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="s">
+    <row r="58" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="2" t="n">
+      <c r="D58" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
+    <row r="59" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="2" t="n">
+      <c r="D59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="s">
+    <row r="60" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="2" t="n">
+      <c r="D60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
+    <row r="61" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="2" t="n">
+      <c r="D61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="s">
+    <row r="62" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="2" t="n">
+      <c r="D62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="s">
+    <row r="63" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" s="2" t="n">
+      <c r="D63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="4" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="s">
+    <row r="64" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E64" s="2" t="n">
+      <c r="D64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
+    <row r="65" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="2" t="n">
+      <c r="D65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="4" t="n">
         <v>180</v>
       </c>
     </row>
@@ -3223,7 +3231,7 @@
         <v>8</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>-135</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3240,7 +3248,7 @@
         <v>8</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3257,7 +3265,7 @@
         <v>8</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,7 +3282,7 @@
         <v>8</v>
       </c>
       <c r="E69" s="2" t="n">
-        <v>-135</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3291,7 +3299,7 @@
         <v>8</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3308,7 +3316,7 @@
         <v>8</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3325,7 +3333,7 @@
         <v>8</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3342,7 +3350,7 @@
         <v>8</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3359,7 +3367,7 @@
         <v>8</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3376,7 +3384,7 @@
         <v>8</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3393,7 +3401,7 @@
         <v>8</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3410,7 +3418,7 @@
         <v>8</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3427,7 +3435,7 @@
         <v>8</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3444,7 +3452,7 @@
         <v>8</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3461,7 +3469,7 @@
         <v>8</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3478,7 +3486,7 @@
         <v>8</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3495,7 +3503,7 @@
         <v>8</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3512,7 +3520,7 @@
         <v>8</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3529,7 +3537,7 @@
         <v>8</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,7 +3554,7 @@
         <v>8</v>
       </c>
       <c r="E85" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3563,7 +3571,7 @@
         <v>8</v>
       </c>
       <c r="E86" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,7 +3588,7 @@
         <v>8</v>
       </c>
       <c r="E87" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3597,7 +3605,7 @@
         <v>8</v>
       </c>
       <c r="E88" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3614,7 +3622,7 @@
         <v>8</v>
       </c>
       <c r="E89" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3631,7 +3639,7 @@
         <v>8</v>
       </c>
       <c r="E90" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3648,7 +3656,7 @@
         <v>8</v>
       </c>
       <c r="E91" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3665,7 +3673,7 @@
         <v>8</v>
       </c>
       <c r="E92" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3682,7 +3690,7 @@
         <v>8</v>
       </c>
       <c r="E93" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3699,7 +3707,7 @@
         <v>8</v>
       </c>
       <c r="E94" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3716,7 +3724,7 @@
         <v>8</v>
       </c>
       <c r="E95" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3733,7 +3741,7 @@
         <v>8</v>
       </c>
       <c r="E96" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3750,7 +3758,7 @@
         <v>8</v>
       </c>
       <c r="E97" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3767,7 +3775,7 @@
         <v>8</v>
       </c>
       <c r="E98" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,7 +3792,7 @@
         <v>8</v>
       </c>
       <c r="E99" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3801,7 +3809,7 @@
         <v>8</v>
       </c>
       <c r="E100" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3818,7 +3826,7 @@
         <v>8</v>
       </c>
       <c r="E101" s="2" t="n">
-        <v>45</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>